<commit_message>
aria ableton max for live
</commit_message>
<xml_diff>
--- a/MIDI Data Generated/Aria Review.xlsx
+++ b/MIDI Data Generated/Aria Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb3f9c8b4bcca75c/Desktop/AUB/Music Intelligence Lab/aria midi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Github Serious\Aria\MIDI Data Generated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="554" documentId="8_{9700EDE2-DBC1-4897-9021-8ABA3D7EA486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE8F2AC2-CCDC-4E5C-B24B-82DC17D8EBBA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CBD9F-4D9D-4751-897E-431327A0A14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{19C7DDBD-3AFA-408D-9C13-A460C79C13F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{19C7DDBD-3AFA-408D-9C13-A460C79C13F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -461,7 +460,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Stability!PivotTable1</c:name>
+    <c:name>[Aria Review.xlsx]Stability!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1730,7 +1729,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Stability!PivotTable2</c:name>
+    <c:name>[Aria Review.xlsx]Stability!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -3331,7 +3330,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Exploration-Minp-Temp!PivotTable2</c:name>
+    <c:name>[Aria Review.xlsx]Exploration-Minp-Temp!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -4148,7 +4147,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Musicality-Temp-Topp!PivotTable3</c:name>
+    <c:name>[Aria Review.xlsx]Musicality-Temp-Topp!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -4841,7 +4840,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Exploration-tenp-minp!PivotTable4</c:name>
+    <c:name>[Aria Review.xlsx]Exploration-tenp-minp!PivotTable4</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -6489,7 +6488,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Exploration3d-temp-minp!PivotTable19</c:name>
+    <c:name>[Aria Review.xlsx]Exploration3d-temp-minp!PivotTable19</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -7274,7 +7273,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Exploration-topp-temp-3d!PivotTable20</c:name>
+    <c:name>[Aria Review.xlsx]Exploration-topp-temp-3d!PivotTable20</c:name>
     <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
@@ -7967,7 +7966,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Aria Review No Hidden ^M Graphs.xlsx]Exploration-topp-temp-3d!PivotTable20</c:name>
+    <c:name>[Aria Review.xlsx]Exploration-topp-temp-3d!PivotTable20</c:name>
     <c:fmtId val="5"/>
   </c:pivotSource>
   <c:chart>
@@ -12900,10 +12899,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15766,8 +15761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB9E970-9003-4965-9EB1-86182E83892C}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18885,7 +18880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89BF9C-263D-4E71-BE3D-1BF3530AFFC0}">
   <dimension ref="A3:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="96" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>